<commit_message>
Initial diagram and fixes
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1_v2.xlsx
+++ b/tests/integration_test_files/simple_1_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68FB89F-6B24-7D4C-A0A9-838DD14A688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECD009-4406-C34F-ACEE-0D427949DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59000" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="586">
   <si>
     <t>Screening</t>
   </si>
@@ -1778,9 +1778,6 @@
   </si>
   <si>
     <t>Dosing</t>
-  </si>
-  <si>
-    <t>D24</t>
   </si>
   <si>
     <t>TIM3</t>
@@ -3429,7 +3426,7 @@
         <v>207</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>195</v>
@@ -5322,7 +5319,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5354,7 +5351,7 @@
         <v>563</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>556</v>
@@ -5380,7 +5377,7 @@
         <v>565</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>219</v>
@@ -5406,7 +5403,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>219</v>
@@ -5445,7 +5442,7 @@
         <v>563</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>556</v>
@@ -5626,7 +5623,7 @@
         <v>549</v>
       </c>
       <c r="B2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5652,10 +5649,10 @@
         <v>561</v>
       </c>
       <c r="B3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D3" t="s">
         <v>550</v>
@@ -5673,21 +5670,21 @@
         <v>560</v>
       </c>
       <c r="I3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C4" t="s">
         <v>565</v>
       </c>
       <c r="D4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E4" t="s">
         <v>563</v>
@@ -5696,65 +5693,65 @@
         <v>563</v>
       </c>
       <c r="G4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F5" t="s">
         <v>563</v>
       </c>
       <c r="G5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H5" t="s">
         <v>560</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C6" t="s">
         <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E6" t="s">
+        <v>577</v>
+      </c>
+      <c r="F6" t="s">
         <v>578</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>579</v>
-      </c>
-      <c r="G6" t="s">
-        <v>580</v>
       </c>
       <c r="H6" t="s">
         <v>560</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add work on decision in timeline
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1_v2.xlsx
+++ b/tests/integration_test_files/simple_1_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECD009-4406-C34F-ACEE-0D427949DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41662568-58F2-B344-8472-FE1413B91E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59000" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="5" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="587">
   <si>
     <t>Screening</t>
   </si>
@@ -1838,6 +1838,9 @@
   </si>
   <si>
     <t>Pre dose</t>
+  </si>
+  <si>
+    <t>(EXIT)</t>
   </si>
 </sst>
 </file>
@@ -1998,10 +2001,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4998,34 +5001,34 @@
       <c r="A3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
@@ -5145,16 +5148,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5319,7 +5322,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5447,7 +5450,9 @@
       <c r="G5" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>

</xml_diff>